<commit_message>
Documentação: Atualização Burndown e 2º Seminário
</commit_message>
<xml_diff>
--- a/Documentação/Burndown.xlsx
+++ b/Documentação/Burndown.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="15255" windowHeight="7935" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="15255" windowHeight="7935" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 3" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint 5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="55">
   <si>
     <t>Tarefas</t>
   </si>
@@ -157,13 +158,31 @@
     <t>Adaptar fase 3</t>
   </si>
   <si>
-    <t>Organizar Trello</t>
-  </si>
-  <si>
     <t>Burndown</t>
   </si>
   <si>
     <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Terminar Fase 1</t>
+  </si>
+  <si>
+    <t>Terminar Fase 2</t>
+  </si>
+  <si>
+    <t>Tela Personagens</t>
+  </si>
+  <si>
+    <t>Implementar barra de informações</t>
+  </si>
+  <si>
+    <t>Mapear botões coord absolutas</t>
+  </si>
+  <si>
+    <t>Objetivos</t>
   </si>
 </sst>
 </file>
@@ -210,36 +229,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="39">
     <dxf>
       <font>
         <condense val="0"/>
@@ -617,35 +607,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
@@ -925,24 +886,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83026304"/>
-        <c:axId val="83027840"/>
+        <c:axId val="75503872"/>
+        <c:axId val="75517952"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="83026304"/>
+        <c:axId val="75503872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd/mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83027840"/>
+        <c:crossAx val="75517952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="83027840"/>
+        <c:axId val="75517952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -951,7 +912,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83026304"/>
+        <c:crossAx val="75503872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -964,7 +925,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1234,24 +1195,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="80749312"/>
-        <c:axId val="133773184"/>
+        <c:axId val="76809344"/>
+        <c:axId val="76810880"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="80749312"/>
+        <c:axId val="76809344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd/mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133773184"/>
+        <c:crossAx val="76810880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="133773184"/>
+        <c:axId val="76810880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1259,7 +1220,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80749312"/>
+        <c:crossAx val="76809344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1272,7 +1233,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1542,24 +1503,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="135617536"/>
-        <c:axId val="107139840"/>
+        <c:axId val="76946816"/>
+        <c:axId val="76952704"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="135617536"/>
+        <c:axId val="76946816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd/mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107139840"/>
+        <c:crossAx val="76952704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="107139840"/>
+        <c:axId val="76952704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1567,7 +1528,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135617536"/>
+        <c:crossAx val="76946816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1580,7 +1541,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1684,46 +1645,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>41</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1804,70 +1765,70 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>41</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37.846153846153847</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.692307692307693</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.53846153846154</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.384615384615387</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.230769230769234</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.07692307692308</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.923076923076927</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.769230769230774</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.61538461538462</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.461538461538467</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.3076923076923137</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.15384615384616</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.2172489379008766E-15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="138101120"/>
-        <c:axId val="138102656"/>
+        <c:axId val="77588352"/>
+        <c:axId val="77589888"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="138101120"/>
+        <c:axId val="77588352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd/mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138102656"/>
+        <c:crossAx val="77589888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="138102656"/>
+        <c:axId val="77589888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1875,7 +1836,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138101120"/>
+        <c:crossAx val="77588352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1888,7 +1849,315 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>'Sprint 5'!$B$1</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>Sprint 5</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 5'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Atual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 5'!$D$2:$Q$2</c:f>
+              <c:numCache>
+                <c:formatCode>dd/mmm</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>41923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41924</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41926</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41927</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41928</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41929</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41930</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41931</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41932</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41933</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41934</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41935</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41936</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 5'!$D$3:$Q$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0" formatCode="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 5'!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Meta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 5'!$D$2:$Q$2</c:f>
+              <c:numCache>
+                <c:formatCode>dd/mmm</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>41923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41924</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41926</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41927</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41928</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41929</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41930</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41931</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41932</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41933</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41934</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41935</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41936</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 5'!$D$4:$Q$4</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.53846153846154</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.07692307692308</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.61538461538462</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.15384615384616</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.692307692307701</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.230769230769241</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.769230769230779</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.307692307692317</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.8461538461538556</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.3846153846153939</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.9230769230769322</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4615384615384706</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.8817841970012523E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="78034048"/>
+        <c:axId val="78035584"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="78034048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="dd/mmm" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78035584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="78035584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78034048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1934,14 +2203,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>740834</xdr:colOff>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>52917</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>328083</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2005,14 +2274,49 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>306915</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>404811</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>179916</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>515470</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>15253</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>71593</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2321,7 +2625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q12"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
@@ -3008,13 +3312,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:Q12">
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="2" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="37" priority="2" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",D5)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3028,8 +3332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q15"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:Q1048576"/>
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3899,854 +4203,6 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:Q12">
-    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="5" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",D5)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="6" operator="equal">
-      <formula>"S"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13:Q21">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="2" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",D13)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
-      <formula>"S"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:Q15"/>
-  <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="4" max="17" width="8.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:17">
-      <c r="B1" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="2:17">
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1">
-        <v>41895</v>
-      </c>
-      <c r="E2" s="1">
-        <v>41896</v>
-      </c>
-      <c r="F2" s="1">
-        <v>41897</v>
-      </c>
-      <c r="G2" s="1">
-        <v>41898</v>
-      </c>
-      <c r="H2" s="1">
-        <v>41899</v>
-      </c>
-      <c r="I2" s="1">
-        <v>41900</v>
-      </c>
-      <c r="J2" s="1">
-        <v>41901</v>
-      </c>
-      <c r="K2" s="1">
-        <v>41902</v>
-      </c>
-      <c r="L2" s="1">
-        <v>41903</v>
-      </c>
-      <c r="M2" s="1">
-        <v>41904</v>
-      </c>
-      <c r="N2" s="1">
-        <v>41905</v>
-      </c>
-      <c r="O2" s="1">
-        <v>41906</v>
-      </c>
-      <c r="P2" s="1">
-        <v>41907</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>41908</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17">
-      <c r="B3" s="2"/>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <f>$D$4-SUMIF(D5:D176,"S",$C5:$C176)</f>
-        <v>28</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:Q3" si="0">$D$4-SUMIF(E5:E176,"S",$C5:$C176)</f>
-        <v>28</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="G3">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="H3">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="I3">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="J3">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="K3">
-        <f>$D$4-SUMIF(K5:K176,"S",$C5:$C176)</f>
-        <v>22</v>
-      </c>
-      <c r="L3">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="M3">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="N3">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="O3">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="P3">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17">
-      <c r="B4" s="2"/>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3">
-        <f>SUM(C5:C134)</f>
-        <v>28</v>
-      </c>
-      <c r="E4" s="3">
-        <f>D4-$D4/13</f>
-        <v>25.846153846153847</v>
-      </c>
-      <c r="F4" s="3">
-        <f t="shared" ref="F4:Q4" si="1">E4-$D4/13</f>
-        <v>23.692307692307693</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="1"/>
-        <v>21.53846153846154</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" si="1"/>
-        <v>19.384615384615387</v>
-      </c>
-      <c r="I4" s="3">
-        <f t="shared" si="1"/>
-        <v>17.230769230769234</v>
-      </c>
-      <c r="J4" s="3">
-        <f t="shared" si="1"/>
-        <v>15.07692307692308</v>
-      </c>
-      <c r="K4" s="3">
-        <f t="shared" si="1"/>
-        <v>12.923076923076927</v>
-      </c>
-      <c r="L4" s="3">
-        <f t="shared" si="1"/>
-        <v>10.769230769230774</v>
-      </c>
-      <c r="M4" s="3">
-        <f t="shared" si="1"/>
-        <v>8.6153846153846203</v>
-      </c>
-      <c r="N4" s="3">
-        <f t="shared" si="1"/>
-        <v>6.461538461538467</v>
-      </c>
-      <c r="O4" s="3">
-        <f t="shared" si="1"/>
-        <v>4.3076923076923137</v>
-      </c>
-      <c r="P4" s="3">
-        <f t="shared" si="1"/>
-        <v>2.15384615384616</v>
-      </c>
-      <c r="Q4" s="3">
-        <f t="shared" si="1"/>
-        <v>6.2172489379008766E-15</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" ht="45">
-      <c r="B5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" ref="E5:Q15" si="2">D5</f>
-        <v>N</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="H5" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="I5" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="J5" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="K5" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="L5" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="M5" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="N5" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="O5" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="P5" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="Q5" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" ht="75">
-      <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="2"/>
-        <v>N</v>
-      </c>
-      <c r="J6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" t="str">
-        <f t="shared" si="2"/>
-        <v>S</v>
-      </c>
-      <c r="L6" t="str">
-        <f t="shared" si="2"/>
-        <v>S</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" si="2"/>
-        <v>S</v>
-      </c>
-      <c r="N6" t="str">
-        <f t="shared" si="2"/>
-        <v>S</v>
-      </c>
-      <c r="O6" t="str">
-        <f t="shared" si="2"/>
-        <v>S</v>
-      </c>
-      <c r="P6" t="str">
-        <f t="shared" si="2"/>
-        <v>S</v>
-      </c>
-      <c r="Q6" t="str">
-        <f t="shared" si="2"/>
-        <v>S</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" ht="30">
-      <c r="B7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" ref="E7:Q7" si="3">D7</f>
-        <v>N</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="3"/>
-        <v>N</v>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" si="3"/>
-        <v>N</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" si="3"/>
-        <v>N</v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="3"/>
-        <v>N</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="3"/>
-        <v>N</v>
-      </c>
-      <c r="K7" t="str">
-        <f t="shared" si="3"/>
-        <v>N</v>
-      </c>
-      <c r="L7" t="str">
-        <f t="shared" si="3"/>
-        <v>N</v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" si="3"/>
-        <v>N</v>
-      </c>
-      <c r="N7" t="str">
-        <f t="shared" si="3"/>
-        <v>N</v>
-      </c>
-      <c r="O7" t="str">
-        <f t="shared" si="3"/>
-        <v>N</v>
-      </c>
-      <c r="P7" t="str">
-        <f t="shared" si="3"/>
-        <v>N</v>
-      </c>
-      <c r="Q7" t="str">
-        <f t="shared" si="3"/>
-        <v>N</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" ht="30">
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" ref="E8:Q8" si="4">D8</f>
-        <v>N</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="4"/>
-        <v>N</v>
-      </c>
-      <c r="G8" t="str">
-        <f t="shared" si="4"/>
-        <v>N</v>
-      </c>
-      <c r="H8" t="str">
-        <f t="shared" si="4"/>
-        <v>N</v>
-      </c>
-      <c r="I8" t="str">
-        <f t="shared" si="4"/>
-        <v>N</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" si="4"/>
-        <v>N</v>
-      </c>
-      <c r="K8" t="str">
-        <f t="shared" si="4"/>
-        <v>N</v>
-      </c>
-      <c r="L8" t="str">
-        <f t="shared" si="4"/>
-        <v>N</v>
-      </c>
-      <c r="M8" t="str">
-        <f t="shared" si="4"/>
-        <v>N</v>
-      </c>
-      <c r="N8" t="str">
-        <f t="shared" si="4"/>
-        <v>N</v>
-      </c>
-      <c r="O8" t="str">
-        <f t="shared" si="4"/>
-        <v>N</v>
-      </c>
-      <c r="P8" t="str">
-        <f t="shared" si="4"/>
-        <v>N</v>
-      </c>
-      <c r="Q8" t="str">
-        <f t="shared" si="4"/>
-        <v>N</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" ht="45">
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" ref="E9:Q9" si="5">D9</f>
-        <v>N</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="5"/>
-        <v>N</v>
-      </c>
-      <c r="G9" t="str">
-        <f t="shared" si="5"/>
-        <v>N</v>
-      </c>
-      <c r="H9" t="str">
-        <f t="shared" si="5"/>
-        <v>N</v>
-      </c>
-      <c r="I9" t="str">
-        <f t="shared" si="5"/>
-        <v>N</v>
-      </c>
-      <c r="J9" t="str">
-        <f t="shared" si="5"/>
-        <v>N</v>
-      </c>
-      <c r="K9" t="str">
-        <f t="shared" si="5"/>
-        <v>N</v>
-      </c>
-      <c r="L9" t="str">
-        <f t="shared" si="5"/>
-        <v>N</v>
-      </c>
-      <c r="M9" t="str">
-        <f t="shared" si="5"/>
-        <v>N</v>
-      </c>
-      <c r="N9" t="str">
-        <f t="shared" si="5"/>
-        <v>N</v>
-      </c>
-      <c r="O9" t="str">
-        <f t="shared" si="5"/>
-        <v>N</v>
-      </c>
-      <c r="P9" t="str">
-        <f t="shared" si="5"/>
-        <v>N</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17">
-      <c r="B10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" ref="E10:Q12" si="6">D10</f>
-        <v>N</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="G10" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="H10" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="J10" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="K10" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="L10" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="M10" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="N10" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="O10" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="P10" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="Q10" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" ht="45">
-      <c r="B11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" ref="E11:Q11" si="7">D11</f>
-        <v>N</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="7"/>
-        <v>N</v>
-      </c>
-      <c r="G11" t="str">
-        <f t="shared" si="7"/>
-        <v>N</v>
-      </c>
-      <c r="H11" t="str">
-        <f t="shared" si="7"/>
-        <v>N</v>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="7"/>
-        <v>N</v>
-      </c>
-      <c r="J11" t="str">
-        <f t="shared" si="7"/>
-        <v>N</v>
-      </c>
-      <c r="K11" t="str">
-        <f t="shared" si="7"/>
-        <v>N</v>
-      </c>
-      <c r="L11" t="str">
-        <f t="shared" si="7"/>
-        <v>N</v>
-      </c>
-      <c r="M11" t="str">
-        <f t="shared" si="7"/>
-        <v>N</v>
-      </c>
-      <c r="N11" t="s">
-        <v>1</v>
-      </c>
-      <c r="O11" t="str">
-        <f t="shared" si="7"/>
-        <v>S</v>
-      </c>
-      <c r="P11" t="str">
-        <f t="shared" si="7"/>
-        <v>S</v>
-      </c>
-      <c r="Q11" t="str">
-        <f t="shared" si="7"/>
-        <v>S</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" ht="30">
-      <c r="B12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="H12" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="J12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="L12" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="M12" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="N12" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="O12" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="P12" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="Q12" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17">
-      <c r="B13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" ref="E13:Q13" si="8">D13</f>
-        <v>N</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="8"/>
-        <v>N</v>
-      </c>
-      <c r="G13" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="K13" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="L13" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="M13" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="N13" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="O13" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="P13" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="Q13" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" ht="30">
-      <c r="B14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" ref="E14:Q14" si="9">D14</f>
-        <v>N</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="9"/>
-        <v>N</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="9"/>
-        <v>N</v>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" si="9"/>
-        <v>N</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="9"/>
-        <v>N</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="9"/>
-        <v>N</v>
-      </c>
-      <c r="K14" t="str">
-        <f t="shared" si="9"/>
-        <v>N</v>
-      </c>
-      <c r="L14" t="s">
-        <v>1</v>
-      </c>
-      <c r="M14" t="str">
-        <f t="shared" si="9"/>
-        <v>S</v>
-      </c>
-      <c r="N14" t="str">
-        <f t="shared" si="9"/>
-        <v>S</v>
-      </c>
-      <c r="O14" t="str">
-        <f t="shared" si="9"/>
-        <v>S</v>
-      </c>
-      <c r="P14" t="str">
-        <f t="shared" si="9"/>
-        <v>S</v>
-      </c>
-      <c r="Q14" t="str">
-        <f t="shared" si="9"/>
-        <v>S</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17">
-      <c r="B15" s="2"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="D5:Q18">
     <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
       <formula>"N"</formula>
     </cfRule>
@@ -4757,7 +4213,7 @@
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:Q15">
+  <conditionalFormatting sqref="D13:Q21">
     <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
@@ -4773,12 +4229,860 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:Q15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="4" max="17" width="8.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17">
+      <c r="B1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>41895</v>
+      </c>
+      <c r="E2" s="1">
+        <v>41896</v>
+      </c>
+      <c r="F2" s="1">
+        <v>41897</v>
+      </c>
+      <c r="G2" s="1">
+        <v>41898</v>
+      </c>
+      <c r="H2" s="1">
+        <v>41899</v>
+      </c>
+      <c r="I2" s="1">
+        <v>41900</v>
+      </c>
+      <c r="J2" s="1">
+        <v>41901</v>
+      </c>
+      <c r="K2" s="1">
+        <v>41902</v>
+      </c>
+      <c r="L2" s="1">
+        <v>41903</v>
+      </c>
+      <c r="M2" s="1">
+        <v>41904</v>
+      </c>
+      <c r="N2" s="1">
+        <v>41905</v>
+      </c>
+      <c r="O2" s="1">
+        <v>41906</v>
+      </c>
+      <c r="P2" s="1">
+        <v>41907</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>41908</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17">
+      <c r="B3" s="2"/>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <f>$D$4-SUMIF(D5:D176,"S",$C5:$C176)</f>
+        <v>28</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:Q3" si="0">$D$4-SUMIF(E5:E176,"S",$C5:$C176)</f>
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="K3">
+        <f>$D$4-SUMIF(K5:K176,"S",$C5:$C176)</f>
+        <v>22</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17">
+      <c r="B4" s="2"/>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3">
+        <f>SUM(C5:C134)</f>
+        <v>28</v>
+      </c>
+      <c r="E4" s="3">
+        <f>D4-$D4/13</f>
+        <v>25.846153846153847</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" ref="F4:Q4" si="1">E4-$D4/13</f>
+        <v>23.692307692307693</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="1"/>
+        <v>21.53846153846154</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>19.384615384615387</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="1"/>
+        <v>17.230769230769234</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="1"/>
+        <v>15.07692307692308</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="1"/>
+        <v>12.923076923076927</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" si="1"/>
+        <v>10.769230769230774</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" si="1"/>
+        <v>8.6153846153846203</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" si="1"/>
+        <v>6.461538461538467</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" si="1"/>
+        <v>4.3076923076923137</v>
+      </c>
+      <c r="P4" s="3">
+        <f t="shared" si="1"/>
+        <v>2.15384615384616</v>
+      </c>
+      <c r="Q4" s="3">
+        <f t="shared" si="1"/>
+        <v>6.2172489379008766E-15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17">
+      <c r="B5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" ref="E5:Q6" si="2">D5</f>
+        <v>N</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="45">
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" ht="30">
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" ref="E7:Q7" si="3">D7</f>
+        <v>N</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="3"/>
+        <v>N</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="3"/>
+        <v>N</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="3"/>
+        <v>N</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="3"/>
+        <v>N</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="3"/>
+        <v>N</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="3"/>
+        <v>N</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="3"/>
+        <v>N</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="3"/>
+        <v>N</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="3"/>
+        <v>N</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="3"/>
+        <v>N</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="3"/>
+        <v>N</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="3"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17">
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" ref="E8:Q8" si="4">D8</f>
+        <v>N</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="4"/>
+        <v>N</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="4"/>
+        <v>N</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="4"/>
+        <v>N</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="4"/>
+        <v>N</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="4"/>
+        <v>N</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="4"/>
+        <v>N</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="4"/>
+        <v>N</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="4"/>
+        <v>N</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="4"/>
+        <v>N</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="4"/>
+        <v>N</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="4"/>
+        <v>N</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="4"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="30">
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" ref="E9:P9" si="5">D9</f>
+        <v>N</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="5"/>
+        <v>N</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="5"/>
+        <v>N</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="5"/>
+        <v>N</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="5"/>
+        <v>N</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="5"/>
+        <v>N</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="5"/>
+        <v>N</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="5"/>
+        <v>N</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="5"/>
+        <v>N</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="5"/>
+        <v>N</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="5"/>
+        <v>N</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="5"/>
+        <v>N</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" ref="E10:Q12" si="6">D10</f>
+        <v>N</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" ht="45">
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" ref="E11:Q11" si="7">D11</f>
+        <v>N</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="7"/>
+        <v>N</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="7"/>
+        <v>N</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="7"/>
+        <v>N</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="7"/>
+        <v>N</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="7"/>
+        <v>N</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="7"/>
+        <v>N</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="7"/>
+        <v>N</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="7"/>
+        <v>N</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" ht="30">
+      <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="6"/>
+        <v>S</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="6"/>
+        <v>S</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="6"/>
+        <v>S</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="6"/>
+        <v>S</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="6"/>
+        <v>S</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="6"/>
+        <v>S</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="6"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17">
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" ref="E13:Q13" si="8">D13</f>
+        <v>N</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="8"/>
+        <v>N</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="8"/>
+        <v>S</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="8"/>
+        <v>S</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="8"/>
+        <v>S</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="8"/>
+        <v>S</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="8"/>
+        <v>S</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="8"/>
+        <v>S</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="8"/>
+        <v>S</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="8"/>
+        <v>S</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="8"/>
+        <v>S</v>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" si="8"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" ht="30">
+      <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" ref="E14:Q14" si="9">D14</f>
+        <v>N</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="9"/>
+        <v>N</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="9"/>
+        <v>N</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="9"/>
+        <v>N</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="9"/>
+        <v>N</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="9"/>
+        <v>N</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="9"/>
+        <v>N</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+      <c r="Q14" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17">
+      <c r="B15" s="2"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D5:Q18">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="5" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",D5)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:Q15">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",D13)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:Q17"/>
+  <dimension ref="B1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4789,7 +5093,7 @@
   <sheetData>
     <row r="1" spans="2:17">
       <c r="B1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="2:17">
@@ -4848,60 +5152,60 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <f>$D$4-SUMIF(D5:D176,"S",$C5:$C176)</f>
-        <v>41</v>
+        <f>$D$4-SUMIF(D5:D175,"S",$C5:$C175)</f>
+        <v>39</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:Q3" si="0">$D$4-SUMIF(E5:E176,"S",$C5:$C176)</f>
-        <v>37</v>
+        <f>$D$4-SUMIF(E5:E175,"S",$C5:$C175)</f>
+        <v>35</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
-        <v>35</v>
+        <f>$D$4-SUMIF(F5:F175,"S",$C5:$C175)</f>
+        <v>33</v>
       </c>
       <c r="G3">
-        <f t="shared" si="0"/>
-        <v>29</v>
+        <f>$D$4-SUMIF(G5:G175,"S",$C5:$C175)</f>
+        <v>27</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
-        <v>27</v>
+        <f>$D$4-SUMIF(H5:H175,"S",$C5:$C175)</f>
+        <v>25</v>
       </c>
       <c r="I3">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <f>$D$4-SUMIF(I5:I175,"S",$C5:$C175)</f>
+        <v>23</v>
       </c>
       <c r="J3">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <f>$D$4-SUMIF(J5:J175,"S",$C5:$C175)</f>
+        <v>23</v>
       </c>
       <c r="K3">
-        <f>$D$4-SUMIF(K5:K176,"S",$C5:$C176)</f>
-        <v>25</v>
+        <f>$D$4-SUMIF(K5:K175,"S",$C5:$C175)</f>
+        <v>23</v>
       </c>
       <c r="L3">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>$D$4-SUMIF(L5:L175,"S",$C5:$C175)</f>
+        <v>18</v>
       </c>
       <c r="M3">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>$D$4-SUMIF(M5:M175,"S",$C5:$C175)</f>
+        <v>18</v>
       </c>
       <c r="N3">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>$D$4-SUMIF(N5:N175,"S",$C5:$C175)</f>
+        <v>18</v>
       </c>
       <c r="O3">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f>$D$4-SUMIF(O5:O175,"S",$C5:$C175)</f>
+        <v>16</v>
       </c>
       <c r="P3">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f>$D$4-SUMIF(P5:P175,"S",$C5:$C175)</f>
+        <v>16</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f>$D$4-SUMIF(Q5:Q175,"S",$C5:$C175)</f>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:17">
@@ -4910,60 +5214,60 @@
         <v>12</v>
       </c>
       <c r="D4" s="3">
-        <f>SUM(C5:C134)</f>
-        <v>41</v>
+        <f>SUM(C5:C133)</f>
+        <v>39</v>
       </c>
       <c r="E4" s="3">
         <f>D4-$D4/13</f>
-        <v>37.846153846153847</v>
+        <v>36</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F4:Q4" si="1">E4-$D4/13</f>
-        <v>34.692307692307693</v>
+        <f t="shared" ref="F4:Q4" si="0">E4-$D4/13</f>
+        <v>33</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" si="1"/>
-        <v>31.53846153846154</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" si="1"/>
-        <v>28.384615384615387</v>
+        <f t="shared" si="0"/>
+        <v>27</v>
       </c>
       <c r="I4" s="3">
-        <f t="shared" si="1"/>
-        <v>25.230769230769234</v>
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" si="1"/>
-        <v>22.07692307692308</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" si="1"/>
-        <v>18.923076923076927</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" si="1"/>
-        <v>15.769230769230774</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" si="1"/>
-        <v>12.61538461538462</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="N4" s="3">
-        <f t="shared" si="1"/>
-        <v>9.461538461538467</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="O4" s="3">
-        <f t="shared" si="1"/>
-        <v>6.3076923076923137</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="P4" s="3">
-        <f t="shared" si="1"/>
-        <v>3.15384615384616</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="Q4" s="3">
-        <f t="shared" si="1"/>
-        <v>6.2172489379008766E-15</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:17" ht="45">
@@ -4980,51 +5284,51 @@
         <v>1</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ref="E5:Q14" si="2">E5</f>
+        <f t="shared" ref="E5:Q7" si="1">E5</f>
         <v>S</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="O5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="P5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="Q5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
     </row>
@@ -5039,55 +5343,55 @@
         <v>2</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" ref="E6:Q8" si="3">D6</f>
+        <f t="shared" ref="E6:Q8" si="2">D6</f>
         <v>N</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="N6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="O6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="P6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="Q6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -5102,54 +5406,54 @@
         <v>2</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>N</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="N7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="O7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="P7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
       <c r="Q7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S</v>
       </c>
     </row>
@@ -5164,55 +5468,55 @@
         <v>2</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="P8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="Q8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -5227,54 +5531,54 @@
         <v>2</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" ref="E9:Q9" si="4">D9</f>
+        <f t="shared" ref="E9:Q9" si="3">D9</f>
         <v>N</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="G9" t="s">
         <v>1</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="O9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="P9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
       <c r="Q9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
     </row>
@@ -5289,54 +5593,54 @@
         <v>2</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" ref="E10:Q10" si="5">D10</f>
+        <f t="shared" ref="E10:Q10" si="4">D10</f>
         <v>N</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
       <c r="H10" t="s">
         <v>1</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="O10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="P10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="Q10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
     </row>
@@ -5351,54 +5655,54 @@
         <v>2</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" ref="E11:Q11" si="6">D11</f>
+        <f t="shared" ref="E11:Q11" si="5">D11</f>
         <v>N</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>N</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>N</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>N</v>
       </c>
       <c r="I11" t="s">
         <v>1</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="O11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="P11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
     </row>
@@ -5413,54 +5717,54 @@
         <v>2</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" ref="E12:Q12" si="7">D12</f>
+        <f t="shared" ref="E12:Q12" si="6">D12</f>
         <v>N</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>N</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>N</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>N</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>N</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>N</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>N</v>
       </c>
       <c r="L12" t="s">
         <v>1</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="O12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="P12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="Q12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
     </row>
@@ -5475,55 +5779,55 @@
         <v>2</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" ref="E13:Q13" si="8">D13</f>
+        <f t="shared" ref="E13:Q13" si="7">D13</f>
         <v>N</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="O13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="P13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
     </row>
@@ -5538,55 +5842,55 @@
         <v>2</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" ref="E14:Q14" si="9">D14</f>
+        <f t="shared" ref="E14:Q14" si="8">D14</f>
         <v>N</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="O14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="P14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="Q14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
     </row>
@@ -5601,55 +5905,55 @@
         <v>2</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" ref="E15:Q15" si="10">D15</f>
+        <f t="shared" ref="E15:Q15" si="9">D15</f>
         <v>N</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="O15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="P15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
     </row>
@@ -5664,151 +5968,782 @@
         <v>2</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" ref="E16:Q17" si="11">D16</f>
+        <f t="shared" ref="E16:Q16" si="10">D16</f>
         <v>N</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="M16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="N16" t="str">
-        <f t="shared" si="11"/>
-        <v>N</v>
-      </c>
-      <c r="O16" t="str">
-        <f t="shared" si="11"/>
-        <v>N</v>
+        <f t="shared" si="10"/>
+        <v>N</v>
+      </c>
+      <c r="O16" t="s">
+        <v>1</v>
       </c>
       <c r="P16" t="str">
-        <f t="shared" si="11"/>
-        <v>N</v>
+        <f t="shared" si="10"/>
+        <v>S</v>
       </c>
       <c r="Q16" t="str">
-        <f t="shared" si="11"/>
-        <v>N</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17" ht="30">
-      <c r="B17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" t="str">
-        <f t="shared" si="11"/>
-        <v>N</v>
-      </c>
-      <c r="F17" t="str">
-        <f t="shared" si="11"/>
-        <v>N</v>
-      </c>
-      <c r="G17" t="str">
-        <f t="shared" si="11"/>
-        <v>N</v>
-      </c>
-      <c r="H17" t="str">
-        <f t="shared" si="11"/>
-        <v>N</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="11"/>
-        <v>N</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="11"/>
-        <v>N</v>
-      </c>
-      <c r="K17" t="str">
-        <f t="shared" si="11"/>
-        <v>N</v>
-      </c>
-      <c r="L17" t="str">
-        <f t="shared" si="11"/>
-        <v>N</v>
-      </c>
-      <c r="M17" t="str">
-        <f t="shared" si="11"/>
-        <v>N</v>
-      </c>
-      <c r="N17" t="str">
-        <f t="shared" si="11"/>
-        <v>N</v>
-      </c>
-      <c r="O17" t="s">
-        <v>1</v>
-      </c>
-      <c r="P17" t="str">
-        <f t="shared" si="11"/>
-        <v>S</v>
-      </c>
-      <c r="Q17" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D5:Q16">
-    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
+  <conditionalFormatting sqref="D5:Q15">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",D5)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:Q14">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+  <conditionalFormatting sqref="D16:Q16">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="5" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",D13)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",D16)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17:Q17">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:Q12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17">
+      <c r="B1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>41923</v>
+      </c>
+      <c r="E2" s="1">
+        <v>41924</v>
+      </c>
+      <c r="F2" s="1">
+        <v>41925</v>
+      </c>
+      <c r="G2" s="1">
+        <v>41926</v>
+      </c>
+      <c r="H2" s="1">
+        <v>41927</v>
+      </c>
+      <c r="I2" s="1">
+        <v>41928</v>
+      </c>
+      <c r="J2" s="1">
+        <v>41929</v>
+      </c>
+      <c r="K2" s="1">
+        <v>41930</v>
+      </c>
+      <c r="L2" s="1">
+        <v>41931</v>
+      </c>
+      <c r="M2" s="1">
+        <v>41932</v>
+      </c>
+      <c r="N2" s="1">
+        <v>41933</v>
+      </c>
+      <c r="O2" s="1">
+        <v>41934</v>
+      </c>
+      <c r="P2" s="1">
+        <v>41935</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>41936</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17">
+      <c r="B3" s="2"/>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3">
+        <f>$D$4-SUMIF(D5:D171,"S",$C5:$C171)</f>
+        <v>32</v>
+      </c>
+      <c r="E3">
+        <f>$D$4-SUMIF(E5:E171,"S",$C5:$C171)</f>
+        <v>32</v>
+      </c>
+      <c r="F3">
+        <f>$D$4-SUMIF(F5:F171,"S",$C5:$C171)</f>
+        <v>26</v>
+      </c>
+      <c r="G3">
+        <f>$D$4-SUMIF(G5:G171,"S",$C5:$C171)</f>
+        <v>26</v>
+      </c>
+      <c r="H3">
+        <f>$D$4-SUMIF(H5:H171,"S",$C5:$C171)</f>
+        <v>24</v>
+      </c>
+      <c r="I3">
+        <f>$D$4-SUMIF(I5:I171,"S",$C5:$C171)</f>
+        <v>23</v>
+      </c>
+      <c r="J3">
+        <f>$D$4-SUMIF(J5:J171,"S",$C5:$C171)</f>
+        <v>23</v>
+      </c>
+      <c r="K3">
+        <f>$D$4-SUMIF(K5:K171,"S",$C5:$C171)</f>
+        <v>23</v>
+      </c>
+      <c r="L3">
+        <f>$D$4-SUMIF(L5:L171,"S",$C5:$C171)</f>
+        <v>17</v>
+      </c>
+      <c r="M3">
+        <f>$D$4-SUMIF(M5:M171,"S",$C5:$C171)</f>
+        <v>14</v>
+      </c>
+      <c r="N3">
+        <f>$D$4-SUMIF(N5:N171,"S",$C5:$C171)</f>
+        <v>14</v>
+      </c>
+      <c r="O3">
+        <f>$D$4-SUMIF(O5:O171,"S",$C5:$C171)</f>
+        <v>14</v>
+      </c>
+      <c r="P3">
+        <f>$D$4-SUMIF(P5:P171,"S",$C5:$C171)</f>
+        <v>3</v>
+      </c>
+      <c r="Q3">
+        <f>$D$4-SUMIF(Q5:Q171,"S",$C5:$C171)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17">
+      <c r="B4" s="2"/>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3">
+        <f>SUM(C5:C129)</f>
+        <v>32</v>
+      </c>
+      <c r="E4" s="3">
+        <f>D4-$D4/13</f>
+        <v>29.53846153846154</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" ref="F4:Q4" si="0">E4-$D4/13</f>
+        <v>27.07692307692308</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>24.61538461538462</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="0"/>
+        <v>22.15384615384616</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="0"/>
+        <v>19.692307692307701</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="0"/>
+        <v>17.230769230769241</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="0"/>
+        <v>14.769230769230779</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" si="0"/>
+        <v>12.307692307692317</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" si="0"/>
+        <v>9.8461538461538556</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" si="0"/>
+        <v>7.3846153846153939</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" si="0"/>
+        <v>4.9230769230769322</v>
+      </c>
+      <c r="P4" s="3">
+        <f t="shared" si="0"/>
+        <v>2.4615384615384706</v>
+      </c>
+      <c r="Q4" s="3">
+        <f t="shared" si="0"/>
+        <v>8.8817841970012523E-15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" ht="30">
+      <c r="B5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" ref="E5" si="1">D5</f>
+        <v>N</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" ref="F5" si="2">E5</f>
+        <v>N</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" ref="G5" si="3">F5</f>
+        <v>N</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" ref="H5" si="4">G5</f>
+        <v>N</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" ref="I5" si="5">H5</f>
+        <v>N</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" ref="J5" si="6">I5</f>
+        <v>N</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" ref="K5" si="7">J5</f>
+        <v>N</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" ref="M5" si="8">L5</f>
+        <v>S</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" ref="N5" si="9">M5</f>
+        <v>S</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" ref="O5" si="10">N5</f>
+        <v>S</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" ref="P5" si="11">O5</f>
+        <v>S</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" ref="Q5" si="12">P5</f>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="30">
+      <c r="B6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" ref="E6:Q6" si="13">D6</f>
+        <v>N</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="13"/>
+        <v>N</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="13"/>
+        <v>N</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="13"/>
+        <v>N</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="13"/>
+        <v>N</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="13"/>
+        <v>N</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="13"/>
+        <v>N</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="13"/>
+        <v>N</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="13"/>
+        <v>N</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="13"/>
+        <v>N</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="13"/>
+        <v>N</v>
+      </c>
+      <c r="P6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="13"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" ht="45">
+      <c r="B7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" ref="E7:E12" si="14">D7</f>
+        <v>N</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" ref="F7:F12" si="15">E7</f>
+        <v>N</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" ref="G7:G12" si="16">F7</f>
+        <v>N</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" ref="H7:H12" si="17">G7</f>
+        <v>N</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" ref="I7:I12" si="18">H7</f>
+        <v>N</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" ref="J7:J12" si="19">I7</f>
+        <v>N</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" ref="K7:K12" si="20">J7</f>
+        <v>N</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" ref="L7:L12" si="21">K7</f>
+        <v>N</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" ref="M7:M12" si="22">L7</f>
+        <v>N</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" ref="N7:N12" si="23">M7</f>
+        <v>N</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" ref="O7:O12" si="24">N7</f>
+        <v>N</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" ref="P7:P12" si="25">O7</f>
+        <v>N</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17">
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="14"/>
+        <v>N</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="16"/>
+        <v>S</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="17"/>
+        <v>S</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="18"/>
+        <v>S</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="19"/>
+        <v>S</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="20"/>
+        <v>S</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="21"/>
+        <v>S</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="22"/>
+        <v>S</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="23"/>
+        <v>S</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="24"/>
+        <v>S</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="25"/>
+        <v>S</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" ref="Q7:Q12" si="26">P8</f>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="45">
+      <c r="B9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="14"/>
+        <v>N</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="17"/>
+        <v>N</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="18"/>
+        <v>N</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="19"/>
+        <v>N</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="20"/>
+        <v>N</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="21"/>
+        <v>N</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="23"/>
+        <v>S</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="24"/>
+        <v>S</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="25"/>
+        <v>S</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="26"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="60">
+      <c r="B10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="14"/>
+        <v>N</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="18"/>
+        <v>S</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="19"/>
+        <v>S</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="20"/>
+        <v>S</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="21"/>
+        <v>S</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="22"/>
+        <v>S</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="23"/>
+        <v>S</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="24"/>
+        <v>S</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="25"/>
+        <v>S</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="26"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" ht="60">
+      <c r="B11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="14"/>
+        <v>N</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="17"/>
+        <v>N</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="19"/>
+        <v>S</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="20"/>
+        <v>S</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="21"/>
+        <v>S</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="22"/>
+        <v>S</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="23"/>
+        <v>S</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="24"/>
+        <v>S</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="25"/>
+        <v>S</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="26"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17">
+      <c r="B12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="14"/>
+        <v>N</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="17"/>
+        <v>N</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="18"/>
+        <v>N</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="19"/>
+        <v>N</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="20"/>
+        <v>N</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="21"/>
+        <v>N</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="22"/>
+        <v>N</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="23"/>
+        <v>N</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="24"/>
+        <v>N</v>
+      </c>
+      <c r="P12" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="26"/>
+        <v>S</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D5:Q12">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",D17)))</formula>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",D5)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Documentação: -Adição do documento de Análise de Valor Agregado -Atualização do BunrDown, Sprint 6
</commit_message>
<xml_diff>
--- a/Documentação/Burndown.xlsx
+++ b/Documentação/Burndown.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="15255" windowHeight="7935" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="15255" windowHeight="7935" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Sprint 3" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint 4" sheetId="4" r:id="rId4"/>
     <sheet name="Sprint 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sprint 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="72">
   <si>
     <t>Tarefas</t>
   </si>
@@ -184,12 +185,66 @@
   <si>
     <t>Objetivos</t>
   </si>
+  <si>
+    <t>Sprint 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribuir e trocar cartas: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar objetivos: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dar opção de jogar com a IA: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">implementar musicas jogo: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tela de ataque: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salvar Jogo: </t>
+  </si>
+  <si>
+    <t>Tela Opções:</t>
+  </si>
+  <si>
+    <t>Coordenadas relativas:</t>
+  </si>
+  <si>
+    <t>Tratar highlight nos botões:</t>
+  </si>
+  <si>
+    <t>botões com design:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design das telas inicial e opções: </t>
+  </si>
+  <si>
+    <t>Enfeitar a barra de informações:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pausa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doc de arquitetura: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fim do jogo </t>
+  </si>
+  <si>
+    <t>Design cartas</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,16 +252,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF141823"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -214,109 +288,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB1BBCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB1BBCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB1BBCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB1BBCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="30">
     <dxf>
       <font>
         <condense val="0"/>
@@ -628,7 +637,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
@@ -886,24 +894,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="75503872"/>
-        <c:axId val="75517952"/>
+        <c:axId val="72637440"/>
+        <c:axId val="72655616"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="75503872"/>
+        <c:axId val="72637440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd/mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75517952"/>
+        <c:crossAx val="72655616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="75517952"/>
+        <c:axId val="72655616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -912,20 +920,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75503872"/>
+        <c:crossAx val="72637440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000036" footer="0.31496062000000036"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -947,7 +954,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
@@ -1195,24 +1201,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76809344"/>
-        <c:axId val="76810880"/>
+        <c:axId val="73144192"/>
+        <c:axId val="73145728"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="76809344"/>
+        <c:axId val="73144192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd/mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76810880"/>
+        <c:crossAx val="73145728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="76810880"/>
+        <c:axId val="73145728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1220,20 +1226,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76809344"/>
+        <c:crossAx val="73144192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000036" footer="0.31496062000000036"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1255,7 +1260,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
@@ -1503,24 +1507,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76946816"/>
-        <c:axId val="76952704"/>
+        <c:axId val="73302400"/>
+        <c:axId val="73303936"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="76946816"/>
+        <c:axId val="73302400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd/mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76952704"/>
+        <c:crossAx val="73303936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="76952704"/>
+        <c:axId val="73303936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1528,20 +1532,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76946816"/>
+        <c:crossAx val="73302400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000036" footer="0.31496062000000036"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1563,7 +1566,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
@@ -1811,24 +1813,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77588352"/>
-        <c:axId val="77589888"/>
+        <c:axId val="73390720"/>
+        <c:axId val="73400704"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="77588352"/>
+        <c:axId val="73390720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd/mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77589888"/>
+        <c:crossAx val="73400704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="77589888"/>
+        <c:axId val="73400704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1836,20 +1838,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77588352"/>
+        <c:crossAx val="73390720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000036" footer="0.31496062000000036"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1871,7 +1872,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
@@ -2119,24 +2119,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="78034048"/>
-        <c:axId val="78035584"/>
+        <c:axId val="73454720"/>
+        <c:axId val="73456256"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="78034048"/>
+        <c:axId val="73454720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd/mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78035584"/>
+        <c:crossAx val="73456256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="78035584"/>
+        <c:axId val="73456256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2144,7 +2144,323 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78034048"/>
+        <c:crossAx val="73454720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000047" footer="0.31496062000000047"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>'Sprint 6'!$B$1</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>Sprint 6</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.42688211557861383"/>
+          <c:y val="1.2040197193780813E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 6'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Atual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 6'!$D$2:$Q$2</c:f>
+              <c:numCache>
+                <c:formatCode>dd/mmm</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>41937</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41938</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41939</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41940</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41941</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41942</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41943</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41944</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41945</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41946</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41947</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41948</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41949</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41950</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 6'!$D$3:$Q$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0" formatCode="0">
+                  <c:v>55.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>51.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 6'!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Meta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 6'!$D$2:$Q$2</c:f>
+              <c:numCache>
+                <c:formatCode>dd/mmm</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>41937</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41938</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41939</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41940</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41941</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41942</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41943</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41944</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41945</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41946</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41947</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41948</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41949</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41950</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 6'!$D$4:$Q$4</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>55.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.230769230769234</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.961538461538467</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42.692307692307701</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.423076923076934</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34.153846153846168</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.884615384615397</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.615384615384627</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.346153846153857</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.076923076923087</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.807692307692317</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.5384615384615472</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.269230769230778</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.8817841970012523E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="75918720"/>
+        <c:axId val="75936896"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="75918720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="dd/mmm" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75936896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="75936896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75918720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2157,7 +2473,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000052" footer="0.31496062000000052"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2333,6 +2649,90 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>110043</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>164025</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>559595</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>59531</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>107156</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conector reto 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="2863454" y="7745016"/>
+          <a:ext cx="2333625" cy="11906"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2621,6 +3021,285 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Escritório">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="1F497D"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="EEECE1"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4F81BD"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="C0504D"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="9BBB59"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="8064A2"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4BACC6"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="F79646"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0000FF"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="800080"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Escritório">
+    <a:majorFont>
+      <a:latin typeface="Cambria"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Escritório">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:shade val="51000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="80000">
+            <a:schemeClr val="phClr">
+              <a:shade val="93000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="94000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q12"/>
@@ -3312,13 +3991,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:Q12">
-    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="2" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="28" priority="2" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",D5)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4203,24 +4882,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:Q12">
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",D5)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:Q21">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",D13)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4233,7 +4912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
@@ -5051,24 +5730,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:Q18">
-    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="5" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",D5)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:Q15">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",D13)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5081,8 +5760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q16"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5152,59 +5831,59 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <f>$D$4-SUMIF(D5:D175,"S",$C5:$C175)</f>
+        <f t="shared" ref="D3:Q3" si="0">$D$4-SUMIF(D5:D175,"S",$C5:$C175)</f>
         <v>39</v>
       </c>
       <c r="E3">
-        <f>$D$4-SUMIF(E5:E175,"S",$C5:$C175)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="F3">
-        <f>$D$4-SUMIF(F5:F175,"S",$C5:$C175)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="G3">
-        <f>$D$4-SUMIF(G5:G175,"S",$C5:$C175)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="H3">
-        <f>$D$4-SUMIF(H5:H175,"S",$C5:$C175)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="I3">
-        <f>$D$4-SUMIF(I5:I175,"S",$C5:$C175)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="J3">
-        <f>$D$4-SUMIF(J5:J175,"S",$C5:$C175)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="K3">
-        <f>$D$4-SUMIF(K5:K175,"S",$C5:$C175)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="L3">
-        <f>$D$4-SUMIF(L5:L175,"S",$C5:$C175)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="M3">
-        <f>$D$4-SUMIF(M5:M175,"S",$C5:$C175)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N3">
-        <f>$D$4-SUMIF(N5:N175,"S",$C5:$C175)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="O3">
-        <f>$D$4-SUMIF(O5:O175,"S",$C5:$C175)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="P3">
-        <f>$D$4-SUMIF(P5:P175,"S",$C5:$C175)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="Q3">
-        <f>$D$4-SUMIF(Q5:Q175,"S",$C5:$C175)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
@@ -5222,51 +5901,51 @@
         <v>36</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F4:Q4" si="0">E4-$D4/13</f>
+        <f t="shared" ref="F4:Q4" si="1">E4-$D4/13</f>
         <v>33</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="I4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="N4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="O4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="P4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="Q4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5284,51 +5963,51 @@
         <v>1</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ref="E5:Q7" si="1">E5</f>
+        <f t="shared" ref="E5:Q7" si="2">E5</f>
         <v>S</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="O5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="P5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="Q5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
     </row>
@@ -5343,55 +6022,55 @@
         <v>2</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" ref="E6:Q8" si="2">D6</f>
+        <f t="shared" ref="E6:Q8" si="3">D6</f>
         <v>N</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="N6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="O6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="P6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="Q6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5406,54 +6085,54 @@
         <v>2</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="N7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="O7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="P7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="Q7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
     </row>
@@ -5468,55 +6147,55 @@
         <v>2</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="P8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
       <c r="Q8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5531,54 +6210,54 @@
         <v>2</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" ref="E9:Q9" si="3">D9</f>
+        <f t="shared" ref="E9:Q9" si="4">D9</f>
         <v>N</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
       <c r="G9" t="s">
         <v>1</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="O9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="P9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="Q9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
     </row>
@@ -5593,54 +6272,54 @@
         <v>2</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" ref="E10:Q10" si="4">D10</f>
+        <f t="shared" ref="E10:Q10" si="5">D10</f>
         <v>N</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>N</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>N</v>
       </c>
       <c r="H10" t="s">
         <v>1</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="O10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="P10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="Q10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
     </row>
@@ -5655,54 +6334,54 @@
         <v>2</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" ref="E11:Q11" si="5">D11</f>
+        <f t="shared" ref="E11:Q11" si="6">D11</f>
         <v>N</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>N</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>N</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>N</v>
       </c>
       <c r="I11" t="s">
         <v>1</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="O11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="P11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
     </row>
@@ -5717,54 +6396,54 @@
         <v>2</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" ref="E12:Q12" si="6">D12</f>
+        <f t="shared" ref="E12:Q12" si="7">D12</f>
         <v>N</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>N</v>
       </c>
       <c r="L12" t="s">
         <v>1</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>S</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>S</v>
       </c>
       <c r="O12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>S</v>
       </c>
       <c r="P12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>S</v>
       </c>
       <c r="Q12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>S</v>
       </c>
     </row>
@@ -5779,55 +6458,55 @@
         <v>2</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" ref="E13:Q13" si="7">D13</f>
+        <f t="shared" ref="E13:Q13" si="8">D13</f>
         <v>N</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="O13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="P13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
     </row>
@@ -5842,55 +6521,55 @@
         <v>2</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" ref="E14:Q14" si="8">D14</f>
+        <f t="shared" ref="E14:Q14" si="9">D14</f>
         <v>N</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="O14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="P14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
       <c r="Q14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>N</v>
       </c>
     </row>
@@ -5905,55 +6584,55 @@
         <v>2</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" ref="E15:Q15" si="9">D15</f>
+        <f t="shared" ref="E15:Q15" si="10">D15</f>
         <v>N</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="O15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="P15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>N</v>
       </c>
     </row>
@@ -5968,77 +6647,77 @@
         <v>2</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" ref="E16:Q16" si="10">D16</f>
+        <f t="shared" ref="E16:Q16" si="11">D16</f>
         <v>N</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>N</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>N</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>N</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>N</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>N</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>N</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>N</v>
       </c>
       <c r="M16" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>N</v>
       </c>
       <c r="N16" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>N</v>
       </c>
       <c r="O16" t="s">
         <v>1</v>
       </c>
       <c r="P16" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>S</v>
       </c>
       <c r="Q16" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>S</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:Q15">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",D5)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:Q16">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",D16)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6051,8 +6730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6121,59 +6800,59 @@
         <v>11</v>
       </c>
       <c r="D3" s="3">
-        <f>$D$4-SUMIF(D5:D171,"S",$C5:$C171)</f>
+        <f t="shared" ref="D3:Q3" si="0">$D$4-SUMIF(D5:D171,"S",$C5:$C171)</f>
         <v>32</v>
       </c>
       <c r="E3">
-        <f>$D$4-SUMIF(E5:E171,"S",$C5:$C171)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="F3">
-        <f>$D$4-SUMIF(F5:F171,"S",$C5:$C171)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="G3">
-        <f>$D$4-SUMIF(G5:G171,"S",$C5:$C171)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="H3">
-        <f>$D$4-SUMIF(H5:H171,"S",$C5:$C171)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="I3">
-        <f>$D$4-SUMIF(I5:I171,"S",$C5:$C171)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="J3">
-        <f>$D$4-SUMIF(J5:J171,"S",$C5:$C171)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="K3">
-        <f>$D$4-SUMIF(K5:K171,"S",$C5:$C171)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="L3">
-        <f>$D$4-SUMIF(L5:L171,"S",$C5:$C171)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="M3">
-        <f>$D$4-SUMIF(M5:M171,"S",$C5:$C171)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="N3">
-        <f>$D$4-SUMIF(N5:N171,"S",$C5:$C171)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="O3">
-        <f>$D$4-SUMIF(O5:O171,"S",$C5:$C171)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="P3">
-        <f>$D$4-SUMIF(P5:P171,"S",$C5:$C171)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="Q3">
-        <f>$D$4-SUMIF(Q5:Q171,"S",$C5:$C171)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6191,51 +6870,51 @@
         <v>29.53846153846154</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F4:Q4" si="0">E4-$D4/13</f>
+        <f t="shared" ref="F4:Q4" si="1">E4-$D4/13</f>
         <v>27.07692307692308</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24.61538461538462</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.15384615384616</v>
       </c>
       <c r="I4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.692307692307701</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.230769230769241</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.769230769230779</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.307692307692317</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.8461538461538556</v>
       </c>
       <c r="N4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.3846153846153939</v>
       </c>
       <c r="O4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.9230769230769322</v>
       </c>
       <c r="P4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.4615384615384706</v>
       </c>
       <c r="Q4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.8817841970012523E-15</v>
       </c>
     </row>
@@ -6250,54 +6929,54 @@
         <v>2</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" ref="E5" si="1">D5</f>
+        <f t="shared" ref="E5" si="2">D5</f>
         <v>N</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ref="F5" si="2">E5</f>
+        <f t="shared" ref="F5" si="3">E5</f>
         <v>N</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" ref="G5" si="3">F5</f>
+        <f t="shared" ref="G5" si="4">F5</f>
         <v>N</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" ref="H5" si="4">G5</f>
+        <f t="shared" ref="H5" si="5">G5</f>
         <v>N</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" ref="I5" si="5">H5</f>
+        <f t="shared" ref="I5" si="6">H5</f>
         <v>N</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" ref="J5" si="6">I5</f>
+        <f t="shared" ref="J5" si="7">I5</f>
         <v>N</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" ref="K5" si="7">J5</f>
+        <f t="shared" ref="K5" si="8">J5</f>
         <v>N</v>
       </c>
       <c r="L5" t="s">
         <v>1</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" ref="M5" si="8">L5</f>
+        <f t="shared" ref="M5" si="9">L5</f>
         <v>S</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" ref="N5" si="9">M5</f>
+        <f t="shared" ref="N5" si="10">M5</f>
         <v>S</v>
       </c>
       <c r="O5" t="str">
-        <f t="shared" ref="O5" si="10">N5</f>
+        <f t="shared" ref="O5" si="11">N5</f>
         <v>S</v>
       </c>
       <c r="P5" t="str">
-        <f t="shared" ref="P5" si="11">O5</f>
+        <f t="shared" ref="P5" si="12">O5</f>
         <v>S</v>
       </c>
       <c r="Q5" t="str">
-        <f t="shared" ref="Q5" si="12">P5</f>
+        <f t="shared" ref="Q5" si="13">P5</f>
         <v>S</v>
       </c>
     </row>
@@ -6312,58 +6991,58 @@
         <v>2</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" ref="E6:Q6" si="13">D6</f>
+        <f t="shared" ref="E6:Q6" si="14">D6</f>
         <v>N</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>N</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>N</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>N</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>N</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>N</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>N</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>N</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>N</v>
       </c>
       <c r="N6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>N</v>
       </c>
       <c r="O6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>N</v>
       </c>
       <c r="P6" t="s">
         <v>1</v>
       </c>
       <c r="Q6" t="str">
-        <f t="shared" si="13"/>
-        <v>S</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" ht="45">
+        <f t="shared" si="14"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" ht="30">
       <c r="B7" s="2" t="s">
         <v>37</v>
       </c>
@@ -6374,51 +7053,51 @@
         <v>2</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" ref="E7:E12" si="14">D7</f>
+        <f t="shared" ref="E7:E12" si="15">D7</f>
         <v>N</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" ref="F7:F12" si="15">E7</f>
+        <f t="shared" ref="F7:F12" si="16">E7</f>
         <v>N</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" ref="G7:G12" si="16">F7</f>
+        <f t="shared" ref="G7:G12" si="17">F7</f>
         <v>N</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" ref="H7:H12" si="17">G7</f>
+        <f t="shared" ref="H7:H12" si="18">G7</f>
         <v>N</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" ref="I7:I12" si="18">H7</f>
+        <f t="shared" ref="I7:I12" si="19">H7</f>
         <v>N</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" ref="J7:J12" si="19">I7</f>
+        <f t="shared" ref="J7:J12" si="20">I7</f>
         <v>N</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" ref="K7:K12" si="20">J7</f>
+        <f t="shared" ref="K7:K12" si="21">J7</f>
         <v>N</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" ref="L7:L12" si="21">K7</f>
+        <f t="shared" ref="L7:L12" si="22">K7</f>
         <v>N</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" ref="M7:M12" si="22">L7</f>
+        <f t="shared" ref="M7:M12" si="23">L7</f>
         <v>N</v>
       </c>
       <c r="N7" t="str">
-        <f t="shared" ref="N7:N12" si="23">M7</f>
+        <f t="shared" ref="N7:N12" si="24">M7</f>
         <v>N</v>
       </c>
       <c r="O7" t="str">
-        <f t="shared" ref="O7:O12" si="24">N7</f>
+        <f t="shared" ref="O7:O12" si="25">N7</f>
         <v>N</v>
       </c>
       <c r="P7" t="str">
-        <f t="shared" ref="P7:P12" si="25">O7</f>
+        <f t="shared" ref="P7:P11" si="26">O7</f>
         <v>N</v>
       </c>
       <c r="Q7" t="s">
@@ -6436,54 +7115,54 @@
         <v>2</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>N</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>S</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>S</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>S</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>S</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>S</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>S</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>S</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>S</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>S</v>
       </c>
       <c r="P8" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>S</v>
       </c>
       <c r="Q8" t="str">
-        <f t="shared" ref="Q7:Q12" si="26">P8</f>
+        <f t="shared" ref="Q8:Q12" si="27">P8</f>
         <v>S</v>
       </c>
     </row>
@@ -6498,54 +7177,54 @@
         <v>2</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>N</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>N</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>N</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>N</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>N</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>N</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>N</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>N</v>
       </c>
       <c r="M9" t="s">
         <v>1</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>S</v>
       </c>
       <c r="O9" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>S</v>
       </c>
       <c r="P9" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>S</v>
       </c>
       <c r="Q9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>S</v>
       </c>
     </row>
@@ -6560,54 +7239,54 @@
         <v>2</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>N</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>N</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>N</v>
       </c>
       <c r="H10" t="s">
         <v>1</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>S</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>S</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>S</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>S</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>S</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>S</v>
       </c>
       <c r="O10" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>S</v>
       </c>
       <c r="P10" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>S</v>
       </c>
       <c r="Q10" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>S</v>
       </c>
     </row>
@@ -6622,54 +7301,54 @@
         <v>2</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>N</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>N</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>N</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>N</v>
       </c>
       <c r="I11" t="s">
         <v>1</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>S</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>S</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>S</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>S</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>S</v>
       </c>
       <c r="O11" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>S</v>
       </c>
       <c r="P11" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>S</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>S</v>
       </c>
     </row>
@@ -6684,54 +7363,54 @@
         <v>2</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>N</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>N</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>N</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>N</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>N</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>N</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>N</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>N</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>N</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>N</v>
       </c>
       <c r="O12" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>N</v>
       </c>
       <c r="P12" t="s">
         <v>1</v>
       </c>
       <c r="Q12" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>S</v>
       </c>
     </row>
@@ -6750,4 +7429,1292 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:Q21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P36" sqref="P36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17">
+      <c r="B1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>41937</v>
+      </c>
+      <c r="E2" s="1">
+        <v>41938</v>
+      </c>
+      <c r="F2" s="1">
+        <v>41939</v>
+      </c>
+      <c r="G2" s="1">
+        <v>41940</v>
+      </c>
+      <c r="H2" s="1">
+        <v>41941</v>
+      </c>
+      <c r="I2" s="1">
+        <v>41942</v>
+      </c>
+      <c r="J2" s="1">
+        <v>41943</v>
+      </c>
+      <c r="K2" s="1">
+        <v>41944</v>
+      </c>
+      <c r="L2" s="1">
+        <v>41945</v>
+      </c>
+      <c r="M2" s="1">
+        <v>41946</v>
+      </c>
+      <c r="N2" s="1">
+        <v>41947</v>
+      </c>
+      <c r="O2" s="1">
+        <v>41948</v>
+      </c>
+      <c r="P2" s="1">
+        <v>41949</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>41950</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17">
+      <c r="B3" s="2"/>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:Q3" si="0">$D$4-SUMIF(D5:D171,"S",$C5:$C171)</f>
+        <v>55.5</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>51.5</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>51.5</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>51.5</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>51.5</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>51.5</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>51.5</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>51.5</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>51.5</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>51.5</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>51.5</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="0"/>
+        <v>51.5</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="0"/>
+        <v>51.5</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="0"/>
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17">
+      <c r="B4" s="2"/>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3">
+        <f>SUM(C5:C129)</f>
+        <v>55.5</v>
+      </c>
+      <c r="E4" s="3">
+        <f>D4-$D4/13</f>
+        <v>51.230769230769234</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" ref="F4:Q4" si="1">E4-$D4/13</f>
+        <v>46.961538461538467</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="1"/>
+        <v>42.692307692307701</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>38.423076923076934</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="1"/>
+        <v>34.153846153846168</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="1"/>
+        <v>29.884615384615397</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="1"/>
+        <v>25.615384615384627</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" si="1"/>
+        <v>21.346153846153857</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" si="1"/>
+        <v>17.076923076923087</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" si="1"/>
+        <v>12.807692307692317</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" si="1"/>
+        <v>8.5384615384615472</v>
+      </c>
+      <c r="P4" s="3">
+        <f t="shared" si="1"/>
+        <v>4.269230769230778</v>
+      </c>
+      <c r="Q4" s="3">
+        <f t="shared" si="1"/>
+        <v>8.8817841970012523E-15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" ht="29.25">
+      <c r="B5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" ref="E5" si="2">D5</f>
+        <v>N</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" ref="F5" si="3">E5</f>
+        <v>N</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" ref="G5" si="4">F5</f>
+        <v>N</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" ref="H5" si="5">G5</f>
+        <v>N</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" ref="I5" si="6">H5</f>
+        <v>N</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" ref="J5" si="7">I5</f>
+        <v>N</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" ref="K5" si="8">J5</f>
+        <v>N</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" ref="L5" si="9">K5</f>
+        <v>N</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" ref="M5" si="10">L5</f>
+        <v>N</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" ref="N5" si="11">M5</f>
+        <v>N</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" ref="O5" si="12">N5</f>
+        <v>N</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" ref="P5" si="13">O5</f>
+        <v>N</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" ref="Q5" si="14">P5</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="29.25">
+      <c r="B6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" ref="E6:E19" si="15">D6</f>
+        <v>N</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F20" si="16">E6</f>
+        <v>N</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" ref="G6:G20" si="17">F6</f>
+        <v>N</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" ref="H6:H20" si="18">G6</f>
+        <v>N</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" ref="I6:I20" si="19">H6</f>
+        <v>N</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" ref="J6:J20" si="20">I6</f>
+        <v>N</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" ref="K6:K20" si="21">J6</f>
+        <v>N</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" ref="L6:L20" si="22">K6</f>
+        <v>N</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" ref="M6:M20" si="23">L6</f>
+        <v>N</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" ref="N6:N20" si="24">M6</f>
+        <v>N</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" ref="O6:O20" si="25">N6</f>
+        <v>N</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" ref="P6:P20" si="26">O6</f>
+        <v>N</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" ref="Q6:Q20" si="27">P6</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" ht="29.25">
+      <c r="B7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="17"/>
+        <v>N</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="18"/>
+        <v>N</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="19"/>
+        <v>N</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="20"/>
+        <v>N</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="21"/>
+        <v>N</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="22"/>
+        <v>N</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="23"/>
+        <v>N</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="24"/>
+        <v>N</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="25"/>
+        <v>N</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="26"/>
+        <v>N</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="27"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" ht="29.25">
+      <c r="B8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="6">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="17"/>
+        <v>N</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="18"/>
+        <v>N</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="19"/>
+        <v>N</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="20"/>
+        <v>N</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="21"/>
+        <v>N</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="22"/>
+        <v>N</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="23"/>
+        <v>N</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="24"/>
+        <v>N</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="25"/>
+        <v>N</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="26"/>
+        <v>N</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="27"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17">
+      <c r="B9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="17"/>
+        <v>N</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="18"/>
+        <v>N</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="19"/>
+        <v>N</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="20"/>
+        <v>N</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="21"/>
+        <v>N</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="22"/>
+        <v>N</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="23"/>
+        <v>N</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="24"/>
+        <v>N</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="25"/>
+        <v>N</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="26"/>
+        <v>N</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="27"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="B10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="6">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="17"/>
+        <v>N</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="18"/>
+        <v>N</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="19"/>
+        <v>N</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="20"/>
+        <v>N</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="21"/>
+        <v>N</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="22"/>
+        <v>N</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="23"/>
+        <v>N</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="24"/>
+        <v>N</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="25"/>
+        <v>N</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="26"/>
+        <v>N</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="27"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="B11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="6">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="17"/>
+        <v>N</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="18"/>
+        <v>N</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="19"/>
+        <v>N</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="20"/>
+        <v>N</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="21"/>
+        <v>N</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="22"/>
+        <v>N</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="23"/>
+        <v>N</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="24"/>
+        <v>N</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="25"/>
+        <v>N</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="26"/>
+        <v>N</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="27"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" ht="29.25">
+      <c r="B12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="17"/>
+        <v>N</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="18"/>
+        <v>N</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="19"/>
+        <v>N</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="20"/>
+        <v>N</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="21"/>
+        <v>N</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="22"/>
+        <v>N</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="23"/>
+        <v>N</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="24"/>
+        <v>N</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="25"/>
+        <v>N</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="26"/>
+        <v>N</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="27"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" ht="29.25">
+      <c r="B13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="17"/>
+        <v>N</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="18"/>
+        <v>N</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="19"/>
+        <v>N</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="20"/>
+        <v>N</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="21"/>
+        <v>N</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="22"/>
+        <v>N</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="23"/>
+        <v>N</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="24"/>
+        <v>N</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="25"/>
+        <v>N</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="26"/>
+        <v>N</v>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" si="27"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" ht="29.25">
+      <c r="B14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="17"/>
+        <v>N</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="18"/>
+        <v>N</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="19"/>
+        <v>N</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="20"/>
+        <v>N</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="21"/>
+        <v>N</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="22"/>
+        <v>N</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="23"/>
+        <v>N</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="24"/>
+        <v>N</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="25"/>
+        <v>N</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="26"/>
+        <v>N</v>
+      </c>
+      <c r="Q14" t="str">
+        <f t="shared" si="27"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" ht="43.5">
+      <c r="B15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="6">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="17"/>
+        <v>N</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="18"/>
+        <v>N</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="19"/>
+        <v>N</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="20"/>
+        <v>N</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="21"/>
+        <v>N</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="22"/>
+        <v>N</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="23"/>
+        <v>N</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="24"/>
+        <v>N</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="25"/>
+        <v>N</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="26"/>
+        <v>N</v>
+      </c>
+      <c r="Q15" t="str">
+        <f t="shared" si="27"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" ht="43.5">
+      <c r="B16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="17"/>
+        <v>N</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="18"/>
+        <v>N</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="19"/>
+        <v>N</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="20"/>
+        <v>N</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="21"/>
+        <v>N</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="22"/>
+        <v>N</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="23"/>
+        <v>N</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="24"/>
+        <v>N</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="25"/>
+        <v>N</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="26"/>
+        <v>N</v>
+      </c>
+      <c r="Q16" t="str">
+        <f t="shared" si="27"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17">
+      <c r="B17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="6">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="17"/>
+        <v>N</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="18"/>
+        <v>N</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="19"/>
+        <v>N</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="20"/>
+        <v>N</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="21"/>
+        <v>N</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="22"/>
+        <v>N</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="23"/>
+        <v>N</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="24"/>
+        <v>N</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="25"/>
+        <v>N</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" si="26"/>
+        <v>N</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" si="27"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" ht="29.25">
+      <c r="B18" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="6">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="16"/>
+        <v>S</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="17"/>
+        <v>S</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="18"/>
+        <v>S</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="19"/>
+        <v>S</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="20"/>
+        <v>S</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="21"/>
+        <v>S</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="22"/>
+        <v>S</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="23"/>
+        <v>S</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="24"/>
+        <v>S</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="25"/>
+        <v>S</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="26"/>
+        <v>S</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="27"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17">
+      <c r="B19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="6">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="15"/>
+        <v>N</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="16"/>
+        <v>N</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="17"/>
+        <v>N</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="18"/>
+        <v>N</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="19"/>
+        <v>N</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="20"/>
+        <v>N</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="21"/>
+        <v>N</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="22"/>
+        <v>N</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="23"/>
+        <v>N</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="24"/>
+        <v>N</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="25"/>
+        <v>N</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="26"/>
+        <v>N</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="27"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17">
+      <c r="B20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="16"/>
+        <v>S</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="17"/>
+        <v>S</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="18"/>
+        <v>S</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="19"/>
+        <v>S</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="20"/>
+        <v>S</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="21"/>
+        <v>S</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="22"/>
+        <v>S</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="23"/>
+        <v>S</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="24"/>
+        <v>S</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="25"/>
+        <v>S</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="26"/>
+        <v>S</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" si="27"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17">
+      <c r="B21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="6">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" ref="F21" si="28">E21</f>
+        <v>S</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" ref="G21" si="29">F21</f>
+        <v>S</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" ref="H21" si="30">G21</f>
+        <v>S</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" ref="I21" si="31">H21</f>
+        <v>S</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" ref="J21" si="32">I21</f>
+        <v>S</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" ref="K21" si="33">J21</f>
+        <v>S</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" ref="L21" si="34">K21</f>
+        <v>S</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" ref="M21" si="35">L21</f>
+        <v>S</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" ref="N21" si="36">M21</f>
+        <v>S</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" ref="O21" si="37">N21</f>
+        <v>S</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" ref="P21" si="38">O21</f>
+        <v>S</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" ref="Q21" si="39">P21</f>
+        <v>S</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D5:Q20">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",D5)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:Q21">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",D21)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>